<commit_message>
Added Schematik of Board
</commit_message>
<xml_diff>
--- a/Berechnung-Timer-Interrupts.xlsx
+++ b/Berechnung-Timer-Interrupts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\Marvin-Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2922A043-C363-4607-8EAA-72D5A7412195}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD5CC39-6ACE-4A22-8B98-01FED99F965B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6765" activeTab="2" xr2:uid="{7BF41FCB-DA09-4529-B0C4-CA2A31262EE2}"/>
   </bookViews>
@@ -382,9 +382,6 @@
     <t>Interrupts per Minute</t>
   </si>
   <si>
-    <t>Interrupts per Second</t>
-  </si>
-  <si>
     <t>Fehler in Counts</t>
   </si>
   <si>
@@ -395,6 +392,9 @@
   </si>
   <si>
     <t>Count (Gerundet)</t>
+  </si>
+  <si>
+    <t>Interrupts per Second [Hz]</t>
   </si>
 </sst>
 </file>
@@ -402,7 +402,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.000E+00"/>
+    <numFmt numFmtId="167" formatCode="0.0E+00"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -515,14 +515,17 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="1" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="1" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20 % - Akzent2" xfId="3" builtinId="34"/>
@@ -1041,7 +1044,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,9 +1071,9 @@
         <f>2^A2</f>
         <v>65536</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <f>B2-A4*A6*1000000/A8</f>
-        <v>60848.5</v>
+        <v>34286</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1080,7 +1083,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1100,7 +1103,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1024</v>
+        <v>256</v>
       </c>
     </row>
   </sheetData>
@@ -1129,16 +1132,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F516793A-69CE-4F6D-9532-CA23EF8EB97E}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
   </cols>
@@ -1154,7 +1157,7 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1163,15 +1166,15 @@
       </c>
       <c r="B2" s="2">
         <f>2^A6</f>
-        <v>256</v>
-      </c>
-      <c r="C2" s="2">
+        <v>65536</v>
+      </c>
+      <c r="C2" s="8">
         <f>B2-B10*A8*1000000/A10</f>
-        <v>255.98914930555554</v>
+        <v>34286</v>
       </c>
       <c r="D2" s="3">
         <f>ABS(C2-C4)</f>
-        <v>1.0850694444457076E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1182,27 +1185,27 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2">
         <f>A2*A4</f>
-        <v>12000</v>
-      </c>
-      <c r="C4" s="6">
+        <v>60</v>
+      </c>
+      <c r="C4" s="5">
         <f>ROUND(C2,0)</f>
-        <v>256</v>
+        <v>34286</v>
       </c>
       <c r="D4" s="4">
         <f>D2/(A6*1000000)</f>
-        <v>1.3563368055571345E-9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1213,20 +1216,20 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2">
         <f>2*B4</f>
-        <v>24000</v>
+        <v>120</v>
       </c>
       <c r="D6" s="3">
         <f>D4*A4</f>
-        <v>2.712673611114269E-7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1234,7 +1237,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1242,8 +1245,8 @@
         <v>16</v>
       </c>
       <c r="B8" s="2">
-        <f>60*B6</f>
-        <v>1440000</v>
+        <f>B6/60</f>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1256,12 +1259,21 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>1024</v>
-      </c>
-      <c r="B10" s="5">
+        <v>256</v>
+      </c>
+      <c r="B10" s="9">
         <f>1/B8</f>
-        <v>6.9444444444444448E-7</v>
-      </c>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="6">
+        <f>B10*A8*1000000</f>
+        <v>8000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D14" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Sync mit Desktop PC
</commit_message>
<xml_diff>
--- a/Berechnung-Timer-Interrupts.xlsx
+++ b/Berechnung-Timer-Interrupts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\Marvin-Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD5CC39-6ACE-4A22-8B98-01FED99F965B}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FF5B33-950C-42C5-8166-342F9584AA2A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6765" activeTab="2" xr2:uid="{7BF41FCB-DA09-4529-B0C4-CA2A31262EE2}"/>
   </bookViews>
@@ -515,7 +515,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
@@ -524,7 +524,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="1" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
@@ -534,7 +533,147 @@
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1018,7 +1157,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1108,7 +1247,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1135,7 +1274,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1162,7 +1301,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="B2" s="2">
         <f>2^A6</f>
@@ -1170,7 +1309,7 @@
       </c>
       <c r="C2" s="8">
         <f>B2-B10*A8*1000000/A10</f>
-        <v>34286</v>
+        <v>62536</v>
       </c>
       <c r="D2" s="3">
         <f>ABS(C2-C4)</f>
@@ -1193,15 +1332,15 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="B4" s="2">
         <f>A2*A4</f>
-        <v>60</v>
+        <v>20000</v>
       </c>
       <c r="C4" s="5">
         <f>ROUND(C2,0)</f>
-        <v>34286</v>
+        <v>62536</v>
       </c>
       <c r="D4" s="4">
         <f>D2/(A6*1000000)</f>
@@ -1225,7 +1364,7 @@
       </c>
       <c r="B6" s="2">
         <f>2*B4</f>
-        <v>120</v>
+        <v>40000</v>
       </c>
       <c r="D6" s="3">
         <f>D4*A4</f>
@@ -1246,7 +1385,7 @@
       </c>
       <c r="B8" s="2">
         <f>B6/60</f>
-        <v>2</v>
+        <v>666.66666666666663</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1259,23 +1398,39 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>256</v>
-      </c>
-      <c r="B10" s="9">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8">
         <f>1/B8</f>
-        <v>0.5</v>
+        <v>1.5E-3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12" s="6">
         <f>B10*A8*1000000</f>
-        <v>8000000</v>
+        <v>24000</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D14" s="7"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
+      <formula>$B$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThanOrEqual">
+      <formula>$B$2</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">

</xml_diff>

<commit_message>
Changed a shitload full of things!
Signed-off-by: Bobbbl <sebastian.draxinger@googlemail.com>
</commit_message>
<xml_diff>
--- a/Berechnung-Timer-Interrupts.xlsx
+++ b/Berechnung-Timer-Interrupts.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\Marvin-Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FF5B33-950C-42C5-8166-342F9584AA2A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FD7C0F-7624-4B9A-B226-78D5C40BB3C3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6765" activeTab="2" xr2:uid="{7BF41FCB-DA09-4529-B0C4-CA2A31262EE2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6765" activeTab="3" xr2:uid="{7BF41FCB-DA09-4529-B0C4-CA2A31262EE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Timer Overflow" sheetId="1" r:id="rId1"/>
     <sheet name="CTC" sheetId="3" r:id="rId2"/>
     <sheet name="RPM in CTC" sheetId="4" r:id="rId3"/>
-    <sheet name="Prescaler" sheetId="2" r:id="rId4"/>
+    <sheet name="Vorschub" sheetId="2" r:id="rId4"/>
+    <sheet name="Auswahlregister" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,6 +27,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -341,7 +343,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Prescale</t>
   </si>
@@ -395,6 +397,48 @@
   </si>
   <si>
     <t>Interrupts per Second [Hz]</t>
+  </si>
+  <si>
+    <t>Vorschub [mm/min]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RPM </t>
+  </si>
+  <si>
+    <t>RPS</t>
+  </si>
+  <si>
+    <t>Bits</t>
+  </si>
+  <si>
+    <t>Steps per Millimeter</t>
+  </si>
+  <si>
+    <t>CPU Freq. [MHz]</t>
+  </si>
+  <si>
+    <t>Schritte pro Minute</t>
+  </si>
+  <si>
+    <t>Interrupts pro Sekunde</t>
+  </si>
+  <si>
+    <t>Round Count</t>
+  </si>
+  <si>
+    <t>Strecke in [mm]</t>
+  </si>
+  <si>
+    <t>Pulsdifferenz</t>
+  </si>
+  <si>
+    <t>Pulse insgesamt</t>
+  </si>
+  <si>
+    <t>Pulsfehler</t>
+  </si>
+  <si>
+    <t>Schrittfehler</t>
   </si>
 </sst>
 </file>
@@ -402,9 +446,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.0E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -447,8 +491,15 @@
       <name val="Segoe UI"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -483,6 +534,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -508,14 +564,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
@@ -523,24 +580,42 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="1" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="20 % - Akzent2" xfId="3" builtinId="34"/>
     <cellStyle name="20 % - Akzent6" xfId="4" builtinId="50"/>
     <cellStyle name="Ausgabe" xfId="2" builtinId="21"/>
+    <cellStyle name="Gut" xfId="5" builtinId="26"/>
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="25">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -550,7 +625,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -601,6 +676,64 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1093,7 +1226,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,7 +1290,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1168,7 +1301,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BE541FEA-F420-44BA-BD62-5763E469512E}">
           <x14:formula1>
-            <xm:f>Prescaler!$A$1:$A$6</xm:f>
+            <xm:f>Auswahlregister!$A$2:$A$6</xm:f>
           </x14:formula1>
           <xm:sqref>A8</xm:sqref>
         </x14:dataValidation>
@@ -1183,7 +1316,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1247,7 +1380,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1259,7 +1392,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F119113C-F1C3-461D-BB40-AF2B7BFB324B}">
           <x14:formula1>
-            <xm:f>Prescaler!$A$1:$A$6</xm:f>
+            <xm:f>Auswahlregister!$A$2:$A$6</xm:f>
           </x14:formula1>
           <xm:sqref>A8</xm:sqref>
         </x14:dataValidation>
@@ -1273,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F516793A-69CE-4F6D-9532-CA23EF8EB97E}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1301,7 +1434,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2">
         <f>2^A6</f>
@@ -1309,7 +1442,7 @@
       </c>
       <c r="C2" s="8">
         <f>B2-B10*A8*1000000/A10</f>
-        <v>62536</v>
+        <v>-84464</v>
       </c>
       <c r="D2" s="3">
         <f>ABS(C2-C4)</f>
@@ -1336,11 +1469,11 @@
       </c>
       <c r="B4" s="2">
         <f>A2*A4</f>
-        <v>20000</v>
+        <v>400</v>
       </c>
       <c r="C4" s="5">
         <f>ROUND(C2,0)</f>
-        <v>62536</v>
+        <v>-84464</v>
       </c>
       <c r="D4" s="4">
         <f>D2/(A6*1000000)</f>
@@ -1364,7 +1497,7 @@
       </c>
       <c r="B6" s="2">
         <f>2*B4</f>
-        <v>40000</v>
+        <v>800</v>
       </c>
       <c r="D6" s="3">
         <f>D4*A4</f>
@@ -1385,7 +1518,7 @@
       </c>
       <c r="B8" s="2">
         <f>B6/60</f>
-        <v>666.66666666666663</v>
+        <v>13.333333333333334</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1402,13 +1535,13 @@
       </c>
       <c r="B10" s="8">
         <f>1/B8</f>
-        <v>1.5E-3</v>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D12" s="6">
         <f>B10*A8*1000000</f>
-        <v>24000</v>
+        <v>1200000</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1416,19 +1549,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
+      <formula>$B$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="lessThan">
       <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
-      <formula>$B$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThanOrEqual">
+      <formula>$B$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
       <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThanOrEqual">
-      <formula>$B$2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1437,7 +1570,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{5E230DF5-F9F3-4F4D-995C-221123C03B06}">
           <x14:formula1>
-            <xm:f>Prescaler!$A$1:$A$6</xm:f>
+            <xm:f>Auswahlregister!$A$2:$A$6</xm:f>
           </x14:formula1>
           <xm:sqref>A10</xm:sqref>
         </x14:dataValidation>
@@ -1449,36 +1582,248 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17151113-6113-4D0C-995E-B82CF71E1647}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>4</v>
+      </c>
+      <c r="B2" s="9">
+        <f>(A2*A4)/A6</f>
+        <v>4</v>
+      </c>
+      <c r="C2" s="9">
+        <f>B6-B12*A10*1*10^6/A12</f>
+        <v>63192.25</v>
+      </c>
+      <c r="D2" s="10">
+        <f>C4-C2</f>
+        <v>-0.25</v>
+      </c>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>200</v>
+      </c>
+      <c r="B4" s="9">
+        <f>B2/60</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="C4" s="9">
+        <f>ROUND(C2,0)</f>
+        <v>63192</v>
+      </c>
+      <c r="D4">
+        <f>A14*A4*2</f>
+        <v>400</v>
+      </c>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>200</v>
+      </c>
+      <c r="B6" s="9">
+        <f>2^A8</f>
+        <v>65536</v>
+      </c>
+      <c r="D6">
+        <f>D4*D2</f>
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>16</v>
+      </c>
+      <c r="B8" s="9">
+        <f>A2*A4</f>
+        <v>800</v>
+      </c>
+      <c r="D8">
+        <f>D6/2</f>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>16</v>
+      </c>
+      <c r="B10" s="9">
+        <f>B8*2/60</f>
+        <v>26.666666666666668</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>256</v>
+      </c>
+      <c r="B12" s="9">
+        <f>1/B10</f>
+        <v>3.7499999999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F2">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThanOrEqual">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThanOrEqual">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{31CBDF14-E874-4269-A598-FA5C622BD28D}">
+          <x14:formula1>
+            <xm:f>Auswahlregister!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>A12</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAC548C-30BC-4945-AB9E-15C123ADB0C9}">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
+      <c r="A1">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>128</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5">
         <v>256</v>
       </c>
     </row>
@@ -1488,6 +1833,7 @@
       </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Work in Progress. Just Update
</commit_message>
<xml_diff>
--- a/Berechnung-Timer-Interrupts.xlsx
+++ b/Berechnung-Timer-Interrupts.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\Marvin-Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12FD7C0F-7624-4B9A-B226-78D5C40BB3C3}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285115CC-0D94-41CB-AE60-56BDF0626205}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6765" activeTab="3" xr2:uid="{7BF41FCB-DA09-4529-B0C4-CA2A31262EE2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6765" activeTab="4" xr2:uid="{7BF41FCB-DA09-4529-B0C4-CA2A31262EE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Timer Overflow" sheetId="1" r:id="rId1"/>
     <sheet name="CTC" sheetId="3" r:id="rId2"/>
     <sheet name="RPM in CTC" sheetId="4" r:id="rId3"/>
     <sheet name="Vorschub" sheetId="2" r:id="rId4"/>
-    <sheet name="Auswahlregister" sheetId="5" r:id="rId5"/>
+    <sheet name="XY Motor" sheetId="6" r:id="rId5"/>
+    <sheet name="Auswahlregister" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -342,8 +343,66 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Sebastian Draxinger</author>
+  </authors>
+  <commentList>
+    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{BA172748-9148-4018-99F7-CAB777E23E97}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sebastian Draxinger:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Steps per Revolution</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{5024039B-90BE-415F-B15C-C971B10CE375}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Sebastian Draxinger:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
   <si>
     <t>Prescale</t>
   </si>
@@ -439,6 +498,84 @@
   </si>
   <si>
     <t>Schrittfehler</t>
+  </si>
+  <si>
+    <t>Punkt 1</t>
+  </si>
+  <si>
+    <t>Punkt 2</t>
+  </si>
+  <si>
+    <t>Res. Vektor</t>
+  </si>
+  <si>
+    <t>Vektoren</t>
+  </si>
+  <si>
+    <t>Winkel</t>
+  </si>
+  <si>
+    <t>Vorschub X</t>
+  </si>
+  <si>
+    <t>Vorschub Y</t>
+  </si>
+  <si>
+    <t>Geschwindigkeiten</t>
+  </si>
+  <si>
+    <t>Zeit X</t>
+  </si>
+  <si>
+    <t>Zeit Y</t>
+  </si>
+  <si>
+    <t>[mm/min]</t>
+  </si>
+  <si>
+    <t>Zeit insgesamt</t>
+  </si>
+  <si>
+    <t>Länge</t>
+  </si>
+  <si>
+    <t>[mm]</t>
+  </si>
+  <si>
+    <t>Count X</t>
+  </si>
+  <si>
+    <t>Count Y</t>
+  </si>
+  <si>
+    <t>CPU Frequ [MHz]</t>
+  </si>
+  <si>
+    <t>Prescaler</t>
+  </si>
+  <si>
+    <t>SPR</t>
+  </si>
+  <si>
+    <t>SPM</t>
+  </si>
+  <si>
+    <t>Timer Bits</t>
+  </si>
+  <si>
+    <t>[min]</t>
+  </si>
+  <si>
+    <t>CMT X</t>
+  </si>
+  <si>
+    <t>CMT Y</t>
+  </si>
+  <si>
+    <t>Round Count X</t>
+  </si>
+  <si>
+    <t>Round Count Y</t>
   </si>
 </sst>
 </file>
@@ -540,7 +677,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -563,6 +700,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -572,7 +720,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
@@ -582,9 +730,21 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="1" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20 % - Akzent2" xfId="3" builtinId="34"/>
@@ -594,7 +754,7 @@
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="25">
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
@@ -690,142 +850,60 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -924,6 +1002,2194 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>687855</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>50520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>687855</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>157020</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Gerader Verbinder 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29853FB1-E070-4C6A-895C-D214EC0F02C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="-5400000">
+          <a:off x="6187680" y="961020"/>
+          <a:ext cx="1440000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="000000">
+            <a:alpha val="75000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>684165</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>127320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>378165</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>127320</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Gerader Verbinder 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BD8FA73-0CA1-4F5F-B370-932ABBB42766}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6903990" y="1651320"/>
+          <a:ext cx="1980000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="000000">
+            <a:alpha val="75000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>666570</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>174784</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>83746</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>165108</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Ellipse 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D10CDDE3-A824-420C-B5A0-C6327DB0DAEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="2143800">
+          <a:off x="6892869" y="1502511"/>
+          <a:ext cx="180000" cy="180000"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E71224">
+            <a:alpha val="75000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="E71224"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="E71224"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>25898</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>32093</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>201185</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>22418</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Ellipse 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A18B6EB5-236D-479F-9C0C-FB9CF6A07B97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11008806" y="420869"/>
+          <a:ext cx="175287" cy="184712"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E71224">
+            <a:alpha val="75000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="E71224"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="E71224"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>592752</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76723</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>284278</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76723</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Gerader Verbinder 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4AFBE999-80CE-42BA-B6BE-3B56362C9AC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="-2113522">
+          <a:off x="6819051" y="1025100"/>
+          <a:ext cx="1980000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="E71224">
+            <a:alpha val="75000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="E71224"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>132181</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>101522</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>132541</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>178234</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="27" name="Freihand 26">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7870A31A-21B2-41BB-A081-4F1FD7242C85}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="11115089" y="490298"/>
+            <a:ext cx="360" cy="76712"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="27" name="Freihand 26">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7870A31A-21B2-41BB-A081-4F1FD7242C85}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11106449" y="481093"/>
+              <a:ext cx="18000" cy="95506"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>125701</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>107687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>154501</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>4412</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="28" name="Freihand 27">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEAAAC1B-30BD-4B4D-9316-2F846176C040}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="11108609" y="690850"/>
+            <a:ext cx="28800" cy="91113"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="28" name="Freihand 27">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEAAAC1B-30BD-4B4D-9316-2F846176C040}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="11099609" y="681359"/>
+              <a:ext cx="46440" cy="109715"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>132181</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>157814</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>155581</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>79378</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="30" name="Freihand 29">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1DC2E09-1A9A-4E07-9119-D26B084B2539}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8646954" y="916515"/>
+            <a:ext cx="23400" cy="111240"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="30" name="Freihand 29">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1DC2E09-1A9A-4E07-9119-D26B084B2539}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8638314" y="907875"/>
+              <a:ext cx="41040" cy="128880"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>156301</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>7063</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>172501</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>93103</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="31" name="Freihand 30">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6A254F6-26F2-42C8-949B-60924728015D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8671074" y="1145115"/>
+            <a:ext cx="16200" cy="86040"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="31" name="Freihand 30">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6A254F6-26F2-42C8-949B-60924728015D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8662434" y="1136115"/>
+              <a:ext cx="33840" cy="103680"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>163141</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>12868</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>163501</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>106828</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="32" name="Freihand 31">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F925BEE6-8F22-4EE7-8941-57FB0E822B19}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8677914" y="1340595"/>
+            <a:ext cx="360" cy="93960"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="32" name="Freihand 31">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F925BEE6-8F22-4EE7-8941-57FB0E822B19}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8669274" y="1331955"/>
+              <a:ext cx="18000" cy="111600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>185101</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>27223</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>185461</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>93463</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="33" name="Freihand 32">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99B8F00D-3474-4738-9795-6F2EFA6AFDBB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8699874" y="1544626"/>
+            <a:ext cx="360" cy="66240"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="33" name="Freihand 32">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99B8F00D-3474-4738-9795-6F2EFA6AFDBB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8690874" y="1535626"/>
+              <a:ext cx="18000" cy="83880"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>683326</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>60571</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>24181</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>60931</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="34" name="Freihand 33">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D60ABE3-59C6-4D9B-A44C-77517A6F5DA0}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="10908122" y="449347"/>
+            <a:ext cx="98967" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="34" name="Freihand 33">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D60ABE3-59C6-4D9B-A44C-77517A6F5DA0}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10899875" y="440707"/>
+              <a:ext cx="115805" cy="18000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>458326</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>58411</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>556966</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>69931</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="35" name="Freihand 34">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42B19A28-8F72-4C81-9997-B9CA8D6E7D78}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="10683122" y="447187"/>
+            <a:ext cx="98640" cy="11520"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="35" name="Freihand 34">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42B19A28-8F72-4C81-9997-B9CA8D6E7D78}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10674122" y="438547"/>
+              <a:ext cx="116280" cy="29160"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>240886</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>67411</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>333766</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>67771</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="36" name="Freihand 35">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE9AF016-71F6-4C98-A191-BF57D6868098}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="10465682" y="456187"/>
+            <a:ext cx="92880" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="36" name="Freihand 35">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE9AF016-71F6-4C98-A191-BF57D6868098}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10456682" y="447187"/>
+              <a:ext cx="110520" cy="18000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>8326</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>42571</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>91486</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>42931</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="37" name="Freihand 36">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B715DE8-5B94-4D0F-9765-9FEDD2CCD265}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="10233122" y="431347"/>
+            <a:ext cx="83160" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="37" name="Freihand 36">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B715DE8-5B94-4D0F-9765-9FEDD2CCD265}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10224482" y="422707"/>
+              <a:ext cx="100800" cy="18000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>582510</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>39329</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>678270</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>48329</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="38" name="Freihand 37">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A14C37F-3233-4E38-B47F-E41CB6E23BA6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="10049194" y="428105"/>
+            <a:ext cx="95760" cy="9000"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="38" name="Freihand 37">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A14C37F-3233-4E38-B47F-E41CB6E23BA6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="10040554" y="419465"/>
+              <a:ext cx="113400" cy="26640"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>382350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>11249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>472350</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>22049</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="39" name="Freihand 38">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFD7546D-A63F-4999-8C18-82682C147C9B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="9849034" y="400025"/>
+            <a:ext cx="90000" cy="10800"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="39" name="Freihand 38">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFD7546D-A63F-4999-8C18-82682C147C9B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9840034" y="391385"/>
+              <a:ext cx="107640" cy="28440"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>153390</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>177525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>303150</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>10889</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="40" name="Freihand 39">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7770A736-9586-4C7D-98F9-DDB273E13418}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="9620074" y="371913"/>
+            <a:ext cx="149760" cy="27752"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="40" name="Freihand 39">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7770A736-9586-4C7D-98F9-DDB273E13418}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9611434" y="361506"/>
+              <a:ext cx="167400" cy="49000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>304935</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>188685</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>61591</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>30552</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="43" name="Freihand 42">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3E559BA-64DA-4C0A-BE9A-BDAD721D086D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="6531234" y="378360"/>
+            <a:ext cx="519480" cy="1169595"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="43" name="Freihand 42">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3E559BA-64DA-4C0A-BE9A-BDAD721D086D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6522152" y="369958"/>
+              <a:ext cx="537280" cy="1186749"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>24855</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>156329</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>235815</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>115378</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId29">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="44" name="Freihand 43">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{932C1B74-AB7E-422A-92F5-8BF5194777DC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="6251154" y="725355"/>
+            <a:ext cx="210960" cy="338400"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="44" name="Freihand 43">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{932C1B74-AB7E-422A-92F5-8BF5194777DC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6242514" y="716355"/>
+              <a:ext cx="228600" cy="356040"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>734055</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>13454</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>379501</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>125548</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId31">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="50" name="Freihand 49">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE1C9A43-02FF-461A-89D1-9CDBC078F28E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="6960354" y="1720532"/>
+            <a:ext cx="1933920" cy="681120"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="50" name="Freihand 49">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE1C9A43-02FF-461A-89D1-9CDBC078F28E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6951354" y="1711892"/>
+              <a:ext cx="1951560" cy="698760"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>329071</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>179640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>645871</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>107729</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId33">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="53" name="Freihand 52">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDE2EBAE-0CDF-46B5-9136-56432C875E11}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7318194" y="1317692"/>
+            <a:ext cx="316800" cy="307440"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="53" name="Freihand 52">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDE2EBAE-0CDF-46B5-9136-56432C875E11}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7309194" y="1309052"/>
+              <a:ext cx="334440" cy="325080"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>643246</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>70098</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1554465" cy="436786"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="Textfeld 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A98C1CE8-49A1-47BF-A426-45AAEF56CD77}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9158019" y="1397825"/>
+          <a:ext cx="1554465" cy="436786"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Winkel zwischen Vektor</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>und X-Achse</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>515127</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>145401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>417933</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>97194</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="Textfeld 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{877293D8-D1D3-4076-A0AA-77A56ECFA346}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5948265" y="1311728"/>
+          <a:ext cx="1545382" cy="534956"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="C00000"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>Alle Achsen</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:t> kommen gleichzeitig an</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>195258</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>151582</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>437372</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="57" name="Gerader Verbinder 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{910BCF94-68BC-4553-A24D-616B02A55D87}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="4870284" y="1317909"/>
+          <a:ext cx="1000226" cy="237193"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="000000">
+            <a:alpha val="75000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="18000">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:tailEnd type="arrow"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2018-11-29T09:04:17.195"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1,'0'199,"0"-199</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink10.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2018-11-29T09:04:36.468"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">230 1,'-219'0,"209"0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink11.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2018-11-29T09:04:37.720"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">266 1,'-27'7,"-1"-1,0-1,1-2,-1-1,-1-1,-26-2,17 0,33 1</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink12.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2018-11-29T09:04:38.369"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">249 29,'-33'0,"9"1,0-1,0-1,0 0,0-2,1-1,-1-1,-16-6,31 7</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink13.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2018-11-29T09:04:39.080"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">416 63,'-73'-18,"-2"2,1 4,-71-3,105 14,32 1</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink14.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2018-11-29T09:04:39.714"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+    <inkml:brush xml:id="br1">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1430 1,'-135'4,"0"7,-13 8,124-16</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br1" timeOffset="18669.293">1029 89,'-11'-4,"-2"0,1 1,0 0,0 1,-1 1,1 0,-1 0,1 2,-1-1,1 2,-1 0,1 0,0 1,0 1,0 0,0 1,-5 3,-4 2,-16 7,1 2,-33 23,57-33,0 0,1 2,0-1,0 1,1 0,1 1,0 1,0-1,-6 14,3-4,1 0,1 1,1 0,1 1,1 0,1 1,1-1,1 1,0 7,3-24,-6 63,3 1,3 1,6 39,12-36,-12-61,-1 1,-1-1,0 1,-1-1,0 7,-2-21,1 32,-1 1,-2-1,-3 10,3-31,-1 0,0-1,0 1,-1-1,-1 0,0 0,0-1,-1 1,0-1,-8 9,6-9,-1 0,-1-1,1 0,-1 0,-1-1,1-1,-1 0,-1 0,1-1,-1 0,0-1,0-1,-1 0,1-1,-2 0,-29 4,1-2,-1-2,-39-3,51 0,26 2,12 3,11 3,17 1,0 2,-1 1,0 2,-1 2,0 1,-1 1,-1 2,-1 1,-1 2,-1 1,7 8,-6 1,-2 2,-1 0,-1 2,-2 0,-2 2,7 19,-21-38,-2 0,0 1,-1-1,-1 1,-1 0,-1-1,-1 15,1-9,0 1,2-1,1 1,2 9,4-3,-3-8,-1-1,-1 1,0 11,-4-26,-1 0,0 0,0-1,-1 1,-1 0,1 0,-1-1,-1 1,0-1,-3 7,-46 87,41-87,1 1,1 1,1 0,0 0,1 0,1 1,1 0,0 0,2 1,0-1,1 3,1 1,1 0,1 1,1-1,2 1,0-1,1-1,6 17,-1-6,-4-13,1 0,0-1,1 0,2 0,-6-12,0 0,1 0,0-1,0 0,1 0,0 0,0-1,0 0,0 0,1 0,0-1,1 1,15 6,0-1,1-1,0-1,1-1,0-1,0-1,0-1,0-2,1 0,-1-2,1-1,-1-1,1-2,10-1</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink15.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2018-11-29T09:05:02.136"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">5 163,'0'25,"0"-1,2 1,1-1,0 0,2 0,3 7,-7-26,0-1,1 0,-1 1,1-1,0 0,0 0,1 0,-1-1,1 1,0 0,-1-1,2 0,-1 0,0 0,1 0,-1 0,1-1,0 1,0-1,0 0,0 0,0-1,0 1,1-1,-1 0,1 0,-1 0,0-1,1 0,-1 1,1-2,-1 1,1 0,-1-1,1 0,-1 0,4-1,12-5,1-1,-1 0,0-1,0-2,-1 0,-1-1,0-1,0 0,-1-1,-1-1,-1-1,11-13,22-31,-2-2,36-66,-144 231,-124 190,144-234,-28 38,4 2,4 3,-26 64,80-145</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink16.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2018-11-29T09:05:40.972"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 122,'1'8,"0"0,1 0,0 0,0 0,0 0,1-1,1 1,-1-1,1 0,0 0,1 0,0 0,5 8,1-1,1-1,0 0,1 0,1 0,-4-5,1-1,0 0,0-1,1 0,0 0,0-1,0-1,1 0,-1 0,13 0,-3 0,1-2,-1-1,1 0,-1-2,21-3,119-37,-48 29,61 2,-8 1,-58 2,1 4,102 12,-157-3,0 1,-1 4,0 2,-1 2,0 2,40 20,-72-27,0 1,-1 1,0 1,-1 0,0 1,-2 2,1-1,-2 2,0 0,-1 2,-1-1,0 1,-2 1,0 1,-1-1,-1 2,-1 0,-1 0,-1 0,0 6,-4-14,1 11,2 0,0-1,2 0,1 0,0-1,4 4,-13-27,1 1,-1-1,1 0,-1 0,1 1,-1-1,1 0,-1 0,1 1,-1-1,1 0,-1 0,1 0,0 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,0 0,-1 0,1-1,-1 1,1 0,-1 0,1-1,-1 1,1 0,-1 0,1-1,-1 1,0-1,1 1,-1 0,1-1,-1 1,0-1,1 1,-1-1,0 1,0-1,1 1,-1-1,0 1,0-1,21-30,-19 27,44-71,-11 17,18-20,-38 58,0 1,2 1,0 1,2 0,14-10,7-1,1 3,1 1,1 2,1 1,1 3,1 2,0 2,4 1,17-2,0 4,0 2,1 3,0 4,33 3,-41 5,1 2,55 16,3 1,69 5,28-5,-133-20,0-3,0-4,74-11,-64 0,0-4,-1-4,14-9,-70 19,-1-2,-1-2,0-1,0-1,-2-2,-1-2,0-1,-1-1,11-12,-27 20,-1 0,0-2,-1 1,0-1,-2-1,0 0,-1-1,3-9,2-6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1979.864">2037 1232,'106'118,"5"-5,13 3,-68-76,-55-39</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2340.657">1937 1892,'92'-116,"5"5,5 4,8 2,-56 53,85-83,83-58,-214 187</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink17.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2018-11-29T09:05:47.732"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">442 1,'22'7,"0"1,0 1,-1 1,0 1,-1 1,0 0,-1 2,0 0,-1 1,-1 1,0 1,-1 0,-1 1,-1 1,0 1,2 4,-2 1,0 1,-2 0,-1 1,-1 0,-1 0,-2 1,0 0,-2 0,-2 1,0 0,-2 5,-1-17,-1 1,-1-1,0 1,-2-1,0 0,0 0,-6 10,6-16,0-1,-1 0,-1 0,1 0,-2 0,1-1,-1 0,-1-1,1 0,-1 0,-1 0,-4 2,-2-3,13-7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="749.569">620 349,'-28'17,"-29"18,-1-2,-56 20,98-46,0-1,-1 0,1-1,-1-2,-1 1,1-2,0 0,-1-1,1-1,-1-1,1 0,0-1,-8-2,13 0,0 0,1 0,-1-1,1-1,-9-5,18 9,-1 1,1 0,-1-1,1 1,0-1,-1 0,1 0,0 0,0 0,1 0,-1 0,0-1,1 1,-1-1,1 1,0-1,0 1,0-1,0 0,0 1,0-1,1 0,-1 0,1 0,0 0,0 1,0-1,0 0,2-1,0 0,0 1,0 0,0-1,0 1,1 0,-1 0,1 0,0 1,0-1,0 1,0-1,0 1,1 0,-1 0,0 0,1 1,0-1,-1 1,5-1,0-1,1 1,0 0,0 0,0 1,0 0,0 1,0 0,6 1,-4 1,-1 0,0 1,1 0,-1 1,0 0,-1 0,1 1,-1 1,0-1,0 1,20 17,-1 0,8 11,-21-19,0 0,1-2,0 1,1-2,1 0,0-2,0 1,14 4,-20-12,1 0,-1-1,1 0,-1 0,1-2,0 1,0-2,-1 0,1 0,0-1,5-2,19-6,-1-1,0-2,3-3,19-10</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2018-11-29T09:04:17.747"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">79 0,'-1'7,"0"0,0-1,-1 1,-1-1,1 1,-1-1,0 0,0 0,0 0,-1 0,-2 2,-21 42,22-37,1 0,1 0,0 0,1 0,1 1,0-1,0 4,1-14</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2018-11-29T09:04:26.370"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">65 1,'0'5,"-1"-1,-1 1,1 0,-1-1,0 1,0-1,0 0,0 0,-1 1,-12 28,4 14,3 1,-1 47,5-60,4-30</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink4.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2018-11-29T09:04:27.055"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">45 0,'0'11,"0"0,0-1,-1 1,0 0,-1-1,0 1,-1-1,0 0,-1 0,-1 3,0-3,1 0,1 0,0 1,0-1,1 1,1 0,0-1,0 1,1 0,0 0,0-7</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink5.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2018-11-29T09:04:27.732"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1,'0'257,"0"-254</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink6.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2018-11-29T09:04:30.816"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 0,'0'171,"0"-159</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink7.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2018-11-29T09:04:34.752"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">288 1,'-282'0,"277"0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink8.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2018-11-29T09:04:35.299"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">273 1,'-33'1,"1"2,-1 2,0 1,2 0,1-2,-2-1,-11-1,37-2</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink9.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2018-11-29T09:04:35.868"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#008C3A"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">257 0,'-250'0,"243"0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C519F60-8A73-4D2F-B692-F112C0A08CED}" name="Tabelle1" displayName="Tabelle1" ref="B2:E4" totalsRowShown="0">
+  <autoFilter ref="B2:E4" xr:uid="{1C6C577C-A1BE-4345-B3F0-CFAB722E6EDB}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{384B947A-E22F-404A-BD0E-2CB2A00706D4}" name="Punkt 1" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{0647A101-5702-4DD0-B566-71162CBFD797}" name="Punkt 2" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{E0A995DF-1ECE-441A-B837-3614EF472942}" name="Res. Vektor" dataDxfId="11">
+      <calculatedColumnFormula>C3-B3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{3A87080C-35C2-4445-A5B5-DA3B02F21FB2}" name="Länge" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C27186F4-D1E8-4CAA-9CFD-F000B738FA85}" name="Tabelle2" displayName="Tabelle2" ref="H2:J4" totalsRowShown="0">
+  <autoFilter ref="H2:J4" xr:uid="{51D7FD7D-4E52-45EB-B577-558A493C39DC}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{6515F90A-4D65-40DF-A6AF-57125513FC2D}" name="Winkel">
+      <calculatedColumnFormula>ACOS((D3*1+D4*0)/(SQRT(D3^2+D4^2)*SQRT(1^2+0^2)))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{7909FC5D-0D48-4DBD-856E-58136F65D002}" name="Vorschub X">
+      <calculatedColumnFormula>COS(H3)*A7</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{639E67CB-8948-4727-A6C7-37D47C208D3B}" name="Vorschub Y">
+      <calculatedColumnFormula>SIN(H3)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1718E89F-7F48-4D7E-839C-EC511988C6BA}" name="Tabelle3" displayName="Tabelle3" ref="C7:E9" totalsRowShown="0">
+  <autoFilter ref="C7:E9" xr:uid="{5ABFAA28-A9C0-400D-B00D-493A00928035}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{EDD25076-4897-48ED-B21C-B8A987D4285A}" name="Zeit X">
+      <calculatedColumnFormula>D3/I4</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{8A26C5D1-B1FC-4ADA-8E1D-448F4A478482}" name="Zeit Y">
+      <calculatedColumnFormula>D4/J4</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{C5548E61-BC28-42E1-9E92-F4F1476A8C11}" name="Zeit insgesamt">
+      <calculatedColumnFormula>E4/A7</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{11B0CA21-1321-408F-AC43-5B77B582BF4C}" name="Tabelle4" displayName="Tabelle4" ref="B13:G14" totalsRowShown="0">
+  <autoFilter ref="B13:G14" xr:uid="{67C55D1B-835A-46C8-AD59-3F994D6B3ABC}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{8AEFBACA-18C4-4995-A37A-965975A51645}" name="Count X">
+      <calculatedColumnFormula>F14*$A$9*10^6/$A$13</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{18832F35-5181-4AFD-B243-4B91817B82D5}" name="Count Y">
+      <calculatedColumnFormula>G14*$A$9*10^6/$A$13</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{B29F7C8A-831C-4C78-A997-03D5A9A68815}" name="Round Count X">
+      <calculatedColumnFormula>ROUND(Tabelle4[Count X],0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{84CA259C-A402-453F-BAB0-3D1EB48C1A08}" name="Round Count Y">
+      <calculatedColumnFormula>ROUND(Tabelle4[Count Y],0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{2EBF021E-6B7D-42F3-BDE9-2918EFF64504}" name="CMT X">
+      <calculatedColumnFormula>C9/($A$17*$D$3*2)*60</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{47912DC6-63DA-440A-9DFD-9964278E4F84}" name="CMT Y">
+      <calculatedColumnFormula>D9/($A$17*$D$4*2)*60</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1584,8 +3850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17151113-6113-4D0C-995E-B82CF71E1647}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1612,23 +3878,23 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>4</v>
-      </c>
-      <c r="B2" s="9">
+      <c r="A2" s="9">
+        <v>10</v>
+      </c>
+      <c r="B2" s="10">
         <f>(A2*A4)/A6</f>
-        <v>4</v>
-      </c>
-      <c r="C2" s="9">
-        <f>B6-B12*A10*1*10^6/A12</f>
-        <v>63192.25</v>
-      </c>
-      <c r="D2" s="10">
+        <v>2</v>
+      </c>
+      <c r="C2" s="10">
+        <f>B12*A10*10^6/A12</f>
+        <v>4687.5</v>
+      </c>
+      <c r="D2" s="11">
         <f>C4-C2</f>
-        <v>-0.25</v>
-      </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+        <v>0.5</v>
+      </c>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1646,21 +3912,21 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>200</v>
-      </c>
-      <c r="B4" s="9">
+        <v>40</v>
+      </c>
+      <c r="B4" s="10">
         <f>B2/60</f>
-        <v>6.6666666666666666E-2</v>
-      </c>
-      <c r="C4" s="9">
-        <f>ROUND(C2,0)</f>
-        <v>63192</v>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="C4" s="10">
+        <f>ROUNDUP(C2,0)</f>
+        <v>4688</v>
       </c>
       <c r="D4">
         <f>A14*A4*2</f>
-        <v>400</v>
-      </c>
-      <c r="F4" s="11"/>
+        <v>160</v>
+      </c>
+      <c r="F4" s="13"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1677,13 +3943,13 @@
       <c r="A6" s="1">
         <v>200</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="10">
         <f>2^A8</f>
         <v>65536</v>
       </c>
       <c r="D6">
         <f>D4*D2</f>
-        <v>-100</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1701,13 +3967,13 @@
       <c r="A8" s="1">
         <v>16</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="10">
         <f>A2*A4</f>
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="D8">
         <f>D6/2</f>
-        <v>-50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1722,9 +3988,13 @@
       <c r="A10" s="1">
         <v>16</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="10">
         <f>B8*2/60</f>
-        <v>26.666666666666668</v>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="D10">
+        <f>0.008078/0.020194</f>
+        <v>0.40001980786372188</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1739,9 +4009,9 @@
       <c r="A12" s="1">
         <v>256</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="10">
         <f>1/B10</f>
-        <v>3.7499999999999999E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1751,7 +4021,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1793,6 +4063,276 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{271D02D4-CFD4-40AB-BA86-81A9FE145DC6}">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="98" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="15"/>
+      <c r="G1" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="12">
+        <v>0</v>
+      </c>
+      <c r="C3" s="12">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12">
+        <f>C3-B3</f>
+        <v>1</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="14"/>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="12">
+        <v>0</v>
+      </c>
+      <c r="C4" s="12">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12">
+        <f>C4-B4</f>
+        <v>1</v>
+      </c>
+      <c r="E4" s="12">
+        <f>SQRT(D3^2+Tabelle1[[#This Row],[Res. Vektor]]^2)</f>
+        <v>1.4142135623730951</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="H4">
+        <f>ACOS((D3*1+D4*0)/(SQRT(D3^2+D4^2)*SQRT(1^2+0^2)))</f>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="I4">
+        <f>COS(H4)*A7</f>
+        <v>84.852813742385706</v>
+      </c>
+      <c r="J4">
+        <f>SIN(H4)*A7</f>
+        <v>84.852813742385692</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>120</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <f>D3/I4</f>
+        <v>1.1785113019775792E-2</v>
+      </c>
+      <c r="D9">
+        <f>D4/J4</f>
+        <v>1.1785113019775794E-2</v>
+      </c>
+      <c r="E9">
+        <f>E4/A7</f>
+        <v>1.1785113019775794E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>256</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F13" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14">
+        <f>F14*$A$9*10^6/$A$13</f>
+        <v>27.621358640099512</v>
+      </c>
+      <c r="C14">
+        <f>G14*$A$9*10^6/$A$13</f>
+        <v>27.621358640099515</v>
+      </c>
+      <c r="D14">
+        <f>ROUND(Tabelle4[Count X],0)</f>
+        <v>28</v>
+      </c>
+      <c r="E14">
+        <f>ROUND(Tabelle4[Count Y],0)</f>
+        <v>28</v>
+      </c>
+      <c r="F14">
+        <f>C9/($A$17*$D$3*2)*60</f>
+        <v>4.4194173824159221E-4</v>
+      </c>
+      <c r="G14">
+        <f>D9/($A$17*$D$4*2)*60</f>
+        <v>4.4194173824159226E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>800</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="G1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <tableParts count="4">
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1C409D2A-91E8-4117-B7D3-A410409ADE36}">
+          <x14:formula1>
+            <xm:f>Auswahlregister!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>A13</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAC548C-30BC-4945-AB9E-15C123ADB0C9}">
   <dimension ref="A1:A6"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updatet Berechnung der Achssynchronisation
</commit_message>
<xml_diff>
--- a/Berechnung-Timer-Interrupts.xlsx
+++ b/Berechnung-Timer-Interrupts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\Marvin-Arduino\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285115CC-0D94-41CB-AE60-56BDF0626205}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE77013B-756C-452E-958D-B4B2BB104ABD}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6765" activeTab="4" xr2:uid="{7BF41FCB-DA09-4529-B0C4-CA2A31262EE2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6165" activeTab="4" xr2:uid="{7BF41FCB-DA09-4529-B0C4-CA2A31262EE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Timer Overflow" sheetId="1" r:id="rId1"/>
@@ -402,7 +402,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
   <si>
     <t>Prescale</t>
   </si>
@@ -576,6 +576,21 @@
   </si>
   <si>
     <t>Round Count Y</t>
+  </si>
+  <si>
+    <t>Fehlerzeit X</t>
+  </si>
+  <si>
+    <t>Fehlerzeit Y</t>
+  </si>
+  <si>
+    <t>deltaX</t>
+  </si>
+  <si>
+    <t>deltaY</t>
+  </si>
+  <si>
+    <t>Fehler in Schritten</t>
   </si>
 </sst>
 </file>
@@ -677,7 +692,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -704,11 +719,44 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -720,7 +768,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
@@ -734,7 +782,9 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -742,9 +792,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="3" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20 % - Akzent2" xfId="3" builtinId="34"/>
@@ -754,7 +806,14 @@
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3118,12 +3177,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8C519F60-8A73-4D2F-B692-F112C0A08CED}" name="Tabelle1" displayName="Tabelle1" ref="B2:E4" totalsRowShown="0">
   <autoFilter ref="B2:E4" xr:uid="{1C6C577C-A1BE-4345-B3F0-CFAB722E6EDB}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{384B947A-E22F-404A-BD0E-2CB2A00706D4}" name="Punkt 1" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{0647A101-5702-4DD0-B566-71162CBFD797}" name="Punkt 2" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{E0A995DF-1ECE-441A-B837-3614EF472942}" name="Res. Vektor" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{384B947A-E22F-404A-BD0E-2CB2A00706D4}" name="Punkt 1" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{0647A101-5702-4DD0-B566-71162CBFD797}" name="Punkt 2" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{E0A995DF-1ECE-441A-B837-3614EF472942}" name="Res. Vektor" dataDxfId="12">
       <calculatedColumnFormula>C3-B3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{3A87080C-35C2-4445-A5B5-DA3B02F21FB2}" name="Länge" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{3A87080C-35C2-4445-A5B5-DA3B02F21FB2}" name="Länge" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3170,10 +3229,10 @@
   <autoFilter ref="B13:G14" xr:uid="{67C55D1B-835A-46C8-AD59-3F994D6B3ABC}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{8AEFBACA-18C4-4995-A37A-965975A51645}" name="Count X">
-      <calculatedColumnFormula>F14*$A$9*10^6/$A$13</calculatedColumnFormula>
+      <calculatedColumnFormula>(C9*60*$A$9*10^6)/($A$17*D3*2*$A$13)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{18832F35-5181-4AFD-B243-4B91817B82D5}" name="Count Y">
-      <calculatedColumnFormula>G14*$A$9*10^6/$A$13</calculatedColumnFormula>
+      <calculatedColumnFormula>(D9*60*$A$9*10^6)/($A$17*D4*2*$A$13)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{B29F7C8A-831C-4C78-A997-03D5A9A68815}" name="Round Count X">
       <calculatedColumnFormula>ROUND(Tabelle4[Count X],0)</calculatedColumnFormula>
@@ -3189,6 +3248,30 @@
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{38922864-5D09-467F-BB77-6CA43630CD65}" name="Tabelle6" displayName="Tabelle6" ref="B16:F17" totalsRowShown="0" tableBorderDxfId="0">
+  <autoFilter ref="B16:F17" xr:uid="{FE042810-1C51-4C62-8E50-8B88FA8B7BCC}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{1F2AB1A3-1F29-4BBA-866B-9A4E8B4F024C}" name="Fehlerzeit X">
+      <calculatedColumnFormula>(Tabelle4[Round Count X]*A17*D3*2*A13)/(60*A9*10^6)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{3EF8F08B-5A91-4619-BF5B-9DC7FE46C6A9}" name="Fehlerzeit Y">
+      <calculatedColumnFormula>(Tabelle4[Round Count Y]*A17*D4*2*A13)/(60*A9*10^6)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{54AA7928-ED0A-4D84-8690-F19061D0D61C}" name="deltaX">
+      <calculatedColumnFormula>C9-B17</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{BC4933E0-89FE-4788-852B-7BE7FF23BD82}" name="deltaY">
+      <calculatedColumnFormula>D9-C17</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{92DF86A0-B728-4E71-9277-149210DBC7A4}" name="Fehler in Schritten">
+      <calculatedColumnFormula>D17/(1.6*10^-5)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -3556,7 +3639,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3646,7 +3729,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3815,18 +3898,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
       <formula>$B$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThanOrEqual">
       <formula>$B$2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3893,8 +3976,8 @@
         <f>C4-C2</f>
         <v>0.5</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -3926,7 +4009,7 @@
         <f>A14*A4*2</f>
         <v>160</v>
       </c>
-      <c r="F4" s="13"/>
+      <c r="F4" s="14"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -4026,22 +4109,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThanOrEqual">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4067,32 +4150,33 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="98" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.85546875" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
     <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="15"/>
-      <c r="G1" s="16" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="17"/>
+      <c r="G1" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -4118,20 +4202,20 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="12">
+      <c r="B3" s="13">
         <v>0</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="13">
         <v>1</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="13">
         <f>C3-B3</f>
         <v>1</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="14"/>
+      <c r="F3" s="16"/>
       <c r="H3" t="s">
         <v>42</v>
       </c>
@@ -4143,42 +4227,42 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="12">
+      <c r="B4" s="13">
         <v>0</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="13">
         <v>1</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="13">
         <f>C4-B4</f>
         <v>1</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="13">
         <f>SQRT(D3^2+Tabelle1[[#This Row],[Res. Vektor]]^2)</f>
         <v>1.4142135623730951</v>
       </c>
-      <c r="F4" s="14"/>
+      <c r="F4" s="16"/>
       <c r="H4">
         <f>ACOS((D3*1+D4*0)/(SQRT(D3^2+D4^2)*SQRT(1^2+0^2)))</f>
         <v>0.78539816339744828</v>
       </c>
       <c r="I4">
         <f>COS(H4)*A7</f>
-        <v>84.852813742385706</v>
+        <v>0.70710678118654757</v>
       </c>
       <c r="J4">
         <f>SIN(H4)*A7</f>
-        <v>84.852813742385692</v>
+        <v>0.70710678118654746</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>120</v>
+      <c r="A7" s="20">
+        <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>40</v>
@@ -4191,7 +4275,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="13" t="s">
         <v>48</v>
       </c>
       <c r="C8" t="s">
@@ -4205,40 +4289,40 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="20">
         <v>16</v>
       </c>
       <c r="C9">
         <f>D3/I4</f>
-        <v>1.1785113019775792E-2</v>
+        <v>1.4142135623730949</v>
       </c>
       <c r="D9">
         <f>D4/J4</f>
-        <v>1.1785113019775794E-2</v>
+        <v>1.4142135623730951</v>
       </c>
       <c r="E9">
         <f>E4/A7</f>
-        <v>1.1785113019775794E-2</v>
+        <v>1.4142135623730951</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="13" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="20">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="13" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>256</v>
+      <c r="A13" s="20">
+        <v>64</v>
       </c>
       <c r="B13" t="s">
         <v>46</v>
@@ -4260,47 +4344,82 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="13" t="s">
         <v>50</v>
       </c>
       <c r="B14">
-        <f>F14*$A$9*10^6/$A$13</f>
-        <v>27.621358640099512</v>
+        <f>(C9*60*$A$9*10^6)/($A$17*D3*2*$A$13)</f>
+        <v>53033.008588991055</v>
       </c>
       <c r="C14">
-        <f>G14*$A$9*10^6/$A$13</f>
-        <v>27.621358640099515</v>
+        <f>(D9*60*$A$9*10^6)/($A$17*D4*2*$A$13)</f>
+        <v>53033.008588991062</v>
       </c>
       <c r="D14">
         <f>ROUND(Tabelle4[Count X],0)</f>
-        <v>28</v>
+        <v>53033</v>
       </c>
       <c r="E14">
         <f>ROUND(Tabelle4[Count Y],0)</f>
-        <v>28</v>
+        <v>53033</v>
       </c>
       <c r="F14">
         <f>C9/($A$17*$D$3*2)*60</f>
-        <v>4.4194173824159221E-4</v>
+        <v>0.21213203435596423</v>
       </c>
       <c r="G14">
         <f>D9/($A$17*$D$4*2)*60</f>
-        <v>4.4194173824159226E-4</v>
+        <v>0.21213203435596426</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>800</v>
+      <c r="A15" s="20">
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="12" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>800</v>
+      <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
+        <v>200</v>
+      </c>
+      <c r="B17">
+        <f>(Tabelle4[Round Count X]*A17*D3*2*A13)/(60*A9*10^6)</f>
+        <v>1.4142133333333333</v>
+      </c>
+      <c r="C17">
+        <f>(Tabelle4[Round Count Y]*A17*D4*2*A13)/(60*A9*10^6)</f>
+        <v>1.4142133333333333</v>
+      </c>
+      <c r="D17">
+        <f>C9-B17</f>
+        <v>2.2903976160115747E-7</v>
+      </c>
+      <c r="E17">
+        <f>D9-C17</f>
+        <v>2.2903976182320207E-7</v>
+      </c>
+      <c r="F17">
+        <f>D17/(1.6*10^-5)</f>
+        <v>1.431498510007234E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4311,11 +4430,12 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
-  <tableParts count="4">
+  <tableParts count="5">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -4337,7 +4457,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4359,7 +4479,7 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>16</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>